<commit_message>
order agnostic binary search and leetcode easy arrays questions
</commit_message>
<xml_diff>
--- a/data-structures-algorithms/practice_sheet.xlsx
+++ b/data-structures-algorithms/practice_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Question Heading</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t xml:space="preserve">solve for O(n) time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotate Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/rotate-image/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add to Array-Form of Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/add-to-array-form-of-integer/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays Medium Questions Community Classroom Assignment</t>
   </si>
 </sst>
 </file>
@@ -183,16 +198,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.96"/>
@@ -266,11 +281,34 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/pascals-triangle-ii/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://leetcode.com/problems/shuffle-the-array/"/>
     <hyperlink ref="B4" r:id="rId3" display="https://leetcode.com/problems/maximum-product-difference-between-two-pairs/"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://leetcode.com/problems/rotate-image/"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://leetcode.com/problems/add-to-array-form-of-integer/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>